<commit_message>
Status counts by group
</commit_message>
<xml_diff>
--- a/data/YGP_Membership_Registration_Sample_Data_Populated.xlsx
+++ b/data/YGP_Membership_Registration_Sample_Data_Populated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jia Ming\Programming_Projects\data-streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D0DF32-05D2-48B5-A165-00C1A62EB1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B8221F-9617-4729-B9C5-EC4D7F6E5ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -149,9 +149,6 @@
     <t>S1234567A</t>
   </si>
   <si>
-    <t>S2345678B</t>
-  </si>
-  <si>
     <t>S3456789C</t>
   </si>
   <si>
@@ -291,9 +288,6 @@
   </si>
   <si>
     <t>Marcus Lee Wai Chun</t>
-  </si>
-  <si>
-    <t>S3863899N</t>
   </si>
   <si>
     <t>European</t>
@@ -749,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -815,28 +809,28 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>10</v>
@@ -863,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>18</v>
@@ -889,7 +883,7 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
@@ -901,40 +895,40 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L2" s="3">
         <v>36851</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q2">
         <v>89898989</v>
       </c>
       <c r="R2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="U2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="V2" s="2">
         <v>44166</v>
@@ -962,7 +956,7 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
         <v>33</v>
@@ -970,44 +964,41 @@
       <c r="H3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L3" s="3">
         <v>36708</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q3">
         <v>89098989</v>
       </c>
       <c r="R3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="S3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V3" s="2">
         <v>42719</v>
@@ -1016,7 +1007,7 @@
         <v>44576</v>
       </c>
       <c r="X3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y3" s="2">
         <v>45245</v>
@@ -1042,7 +1033,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>34</v>
@@ -1051,43 +1042,43 @@
         <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L4" s="3">
         <v>36650</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q4">
         <v>90673289</v>
       </c>
       <c r="R4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V4" s="2">
         <v>45280</v>
@@ -1096,7 +1087,7 @@
         <v>45292</v>
       </c>
       <c r="X4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y4" s="2">
         <v>45250</v>
@@ -1109,67 +1100,64 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
         <v>81</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="2">
         <v>45297</v>
       </c>
       <c r="E5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
         <v>84</v>
-      </c>
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
-        <v>86</v>
-      </c>
       <c r="J5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="3">
         <v>36773</v>
       </c>
       <c r="M5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="N5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q5">
         <v>90283892</v>
       </c>
       <c r="R5" t="s">
+        <v>88</v>
+      </c>
+      <c r="S5" t="s">
+        <v>88</v>
+      </c>
+      <c r="T5" t="s">
+        <v>89</v>
+      </c>
+      <c r="U5" t="s">
         <v>90</v>
-      </c>
-      <c r="S5" t="s">
-        <v>90</v>
-      </c>
-      <c r="T5" t="s">
-        <v>91</v>
-      </c>
-      <c r="U5" t="s">
-        <v>92</v>
       </c>
       <c r="V5" s="2">
         <v>44915</v>
@@ -1178,7 +1166,7 @@
         <v>45292</v>
       </c>
       <c r="X5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y5" s="2">
         <v>45301</v>
@@ -1190,67 +1178,67 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="2">
         <v>45298</v>
       </c>
       <c r="E6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H6" t="s">
         <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L6" s="3">
         <v>36774</v>
       </c>
       <c r="M6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q6">
         <v>90265493</v>
       </c>
       <c r="R6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="S6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="T6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="U6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="V6" s="2">
         <v>44915</v>
@@ -1259,7 +1247,7 @@
         <v>45292</v>
       </c>
       <c r="X6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y6" s="2">
         <v>45301</v>
@@ -1271,13 +1259,13 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" t="s">
         <v>104</v>
-      </c>
-      <c r="B7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" t="s">
-        <v>106</v>
       </c>
       <c r="D7" s="2">
         <v>45298</v>
@@ -1286,52 +1274,52 @@
         <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
         <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" s="3">
         <v>36774</v>
       </c>
       <c r="M7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q7">
         <v>90372493</v>
       </c>
       <c r="R7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="T7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="V7" s="2">
         <v>44885</v>
@@ -1340,7 +1328,7 @@
         <v>45292</v>
       </c>
       <c r="X7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y7" s="2">
         <v>45301</v>
@@ -1353,5 +1341,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Distrution by area and referral count
</commit_message>
<xml_diff>
--- a/data/YGP_Membership_Registration_Sample_Data_Populated.xlsx
+++ b/data/YGP_Membership_Registration_Sample_Data_Populated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jia Ming\Programming_Projects\data-streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27CA41EA-A43F-45FD-935E-7714965BF262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994EA4DE-5B78-4298-8FAF-F34492A6CC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="113">
   <si>
     <t>Name</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>15 (2024)</t>
+  </si>
+  <si>
+    <t>Referral Date (Date received)</t>
   </si>
 </sst>
 </file>
@@ -401,12 +404,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -436,13 +445,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -779,39 +794,39 @@
     <col min="24" max="24" width="36.26953125" customWidth="1"/>
     <col min="25" max="25" width="40.453125" customWidth="1"/>
     <col min="26" max="27" width="35.08984375" customWidth="1"/>
-    <col min="28" max="28" width="35.6328125" customWidth="1"/>
-    <col min="29" max="29" width="29" customWidth="1"/>
+    <col min="28" max="29" width="35.6328125" customWidth="1"/>
+    <col min="30" max="30" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -820,7 +835,7 @@
       <c r="L1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>55</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -841,38 +856,41 @@
       <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="4" t="s">
         <v>17</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -944,8 +962,11 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
+      <c r="AC2" s="2">
+        <v>44166</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1021,8 +1042,11 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
+      <c r="AC3" s="2">
+        <v>44166</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1103,8 +1127,9 @@
       </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -1182,7 +1207,7 @@
       </c>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -1262,8 +1287,11 @@
         <v>45574</v>
       </c>
       <c r="AA6" s="2"/>
+      <c r="AC6" s="2">
+        <v>44166</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>98</v>
       </c>

</xml_diff>